<commit_message>
First upload a file to the Madhu-BCS
</commit_message>
<xml_diff>
--- a/START_STOPvm/Infra_CMDB_Template.xlsx
+++ b/START_STOPvm/Infra_CMDB_Template.xlsx
@@ -157,13 +157,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -215,19 +215,19 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">

</xml_diff>